<commit_message>
ajuste para secondStatus e firstStatus
</commit_message>
<xml_diff>
--- a/ficha.xlsx
+++ b/ficha.xlsx
@@ -444,9 +444,6 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -467,9 +464,6 @@
       <c r="F3">
         <v>6</v>
       </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -488,9 +482,6 @@
         <v>MOVEL</v>
       </c>
       <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "ajuste para secondStatus e firstStatus"
This reverts commit 6c824c2f8904d28a53fd507a3f1ab0be09bc3e9b.
</commit_message>
<xml_diff>
--- a/ficha.xlsx
+++ b/ficha.xlsx
@@ -444,6 +444,9 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -464,6 +467,9 @@
       <c r="F3">
         <v>6</v>
       </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -482,6 +488,9 @@
         <v>MOVEL</v>
       </c>
       <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>6</v>
       </c>
     </row>

</xml_diff>